<commit_message>
#10445 - Adiciona coluna dedepartamento no arquivo
</commit_message>
<xml_diff>
--- a/src/test/resources/arquivo_usuario/planilha_invertida.xlsx
+++ b/src/test/resources/arquivo_usuario/planilha_invertida.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Dados" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'CRIAÇÃO DE USUARIO CONEXAO'!$A$1:$G$651</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'CRIAÇÃO DE USUARIO CONEXAO'!$A$1:$H$651</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t xml:space="preserve">NIVEL/CANAL</t>
   </si>
@@ -32,6 +32,9 @@
     <t xml:space="preserve">CARGO</t>
   </si>
   <si>
+    <t xml:space="preserve">DEPARTAMENTO</t>
+  </si>
+  <si>
     <t xml:space="preserve">CPF</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
     <t xml:space="preserve">VENDEDOR</t>
   </si>
   <si>
+    <t xml:space="preserve">AGENTE_AUTORIZADO   </t>
+  </si>
+  <si>
     <t xml:space="preserve">033.785.690-77</t>
   </si>
   <si>
@@ -60,6 +66,9 @@
   </si>
   <si>
     <t xml:space="preserve">marcelo@mohmal.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   COMERCIAL     </t>
   </si>
   <si>
     <t xml:space="preserve">001.156.850-06</t>
@@ -110,7 +119,7 @@
     <numFmt numFmtId="165" formatCode="000000000\-00"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -141,6 +150,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -163,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -185,13 +202,6 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -217,11 +227,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -246,27 +256,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -590,26 +596,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="48.1938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="13" min="8" style="2" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1023" min="16" style="2" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="2" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="2" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -619,79 +624,79 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="10" t="n">
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="9" t="n">
         <v>38484</v>
       </c>
-      <c r="G2" s="11" t="n">
+      <c r="H2" s="10" t="n">
         <v>4599472608</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="10" t="n">
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="9" t="n">
         <v>38484</v>
       </c>
-      <c r="G3" s="11" t="n">
+      <c r="H3" s="10" t="n">
         <v>4599472608</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D349">
+  <conditionalFormatting sqref="E349">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -699,12 +704,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D349">
+  <conditionalFormatting sqref="E349">
     <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D349">
+  <conditionalFormatting sqref="E349">
     <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>0</formula>
     </cfRule>
@@ -712,12 +717,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D349">
+  <conditionalFormatting sqref="E349">
     <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D349">
+  <conditionalFormatting sqref="E349">
     <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>0</formula>
     </cfRule>
@@ -725,17 +730,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D349">
+  <conditionalFormatting sqref="E349">
     <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D349">
+  <conditionalFormatting sqref="E349">
     <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D349">
+  <conditionalFormatting sqref="E349">
     <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>0</formula>
     </cfRule>
@@ -743,12 +748,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D563">
+  <conditionalFormatting sqref="E563">
     <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D563">
+  <conditionalFormatting sqref="E563">
     <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>0</formula>
     </cfRule>
@@ -756,7 +761,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D563">
+  <conditionalFormatting sqref="E563">
     <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>0</formula>
     </cfRule>
@@ -764,12 +769,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D563">
+  <conditionalFormatting sqref="E563">
     <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D563">
+  <conditionalFormatting sqref="E563">
     <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>0</formula>
     </cfRule>
@@ -777,17 +782,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D563">
+  <conditionalFormatting sqref="E563">
     <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D563">
+  <conditionalFormatting sqref="E563">
     <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D563">
+  <conditionalFormatting sqref="E563">
     <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
       <formula>0</formula>
     </cfRule>
@@ -796,8 +801,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="marcelo@mohmal.com"/>
-    <hyperlink ref="E3" r:id="rId2" display="marcelooliva@mailna.biz"/>
+    <hyperlink ref="F2" r:id="rId1" display="marcelo@mohmal.com"/>
+    <hyperlink ref="F3" r:id="rId2" display="marcelooliva@mailna.biz"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -822,64 +827,67 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>